<commit_message>
Updates to code and figures
</commit_message>
<xml_diff>
--- a/Aim1/figures/scenarios.xlsx
+++ b/Aim1/figures/scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6270a8f4b8f62cae/mcook/aspen-fire/Aim1/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6EBBCED-FD04-F142-825D-80C8C79E5676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{D6EBBCED-FD04-F142-825D-80C8C79E5676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CBBAE46-CF2D-A54D-B921-8895CC260CF4}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{E5C69BA5-0629-ED4B-AF34-D3BDAA73088F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Combined_S1_S2    </t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>Number of Features</t>
-  </si>
-  <si>
-    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -88,9 +85,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -102,9 +99,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -134,24 +136,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,126 +487,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A81BF6-905B-0742-8812-C0D39FE52923}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="4"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="B2" s="11">
         <v>55</v>
       </c>
-      <c r="D2" s="4">
+      <c r="C2" s="6">
         <v>0.91425000000000001</v>
       </c>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4">
+      <c r="B3" s="11"/>
+      <c r="C3" s="6">
         <v>0.90525100000000003</v>
       </c>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4">
+      <c r="B4" s="11"/>
+      <c r="C4" s="6">
         <v>0.84209500000000004</v>
       </c>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="4">
+      <c r="B5" s="11"/>
+      <c r="C5" s="6">
         <v>0.83721400000000001</v>
       </c>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="4">
+      <c r="B6" s="11"/>
+      <c r="C6" s="6">
         <v>0.81980600000000003</v>
       </c>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4">
+      <c r="B7" s="11"/>
+      <c r="C7" s="6">
         <v>0.80493400000000004</v>
       </c>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4">
+      <c r="B8" s="11"/>
+      <c r="C8" s="6">
         <v>0.55744499999999997</v>
       </c>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="4">
+      <c r="B9" s="11"/>
+      <c r="C9" s="6">
         <v>0.485684</v>
       </c>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="4">
+      <c r="B10" s="11"/>
+      <c r="C10" s="6">
         <v>0.462945</v>
       </c>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="4">
+      <c r="B11" s="11"/>
+      <c r="C11" s="6">
         <v>0.45313799999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6">
+      <c r="B12" s="12"/>
+      <c r="C12" s="9">
         <v>0.406495</v>
       </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>